<commit_message>
update diagram and tasks
</commit_message>
<xml_diff>
--- a/Разделение задач.xlsx
+++ b/Разделение задач.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F371EEAE-7158-4509-8E10-B97C083A47BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,12 +29,6 @@
     <t>Гончаров Г.</t>
   </si>
   <si>
-    <t>Гарицай Г.</t>
-  </si>
-  <si>
-    <t>Модель ЗУР (ракета)</t>
-  </si>
-  <si>
     <t>Дамарад В.</t>
   </si>
   <si>
@@ -53,12 +48,18 @@
   </si>
   <si>
     <t>Участник</t>
+  </si>
+  <si>
+    <t>Грицай Г.</t>
+  </si>
+  <si>
+    <t>ПБУ, ПУ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,7 +96,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -111,9 +112,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -151,7 +152,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -186,6 +187,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -221,9 +239,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -396,71 +431,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="35.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>